<commit_message>
Refactor and validate test template
</commit_message>
<xml_diff>
--- a/test/TestConditions.xlsx
+++ b/test/TestConditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\src\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B85CB22-E969-4389-96F5-2470F79FB9DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96977D-BE29-4091-9FF4-BB193644AF2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
   </bookViews>
@@ -379,12 +379,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,6 +390,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,10 +974,10 @@
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="41"/>
       <c r="Z7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1055,10 +1055,10 @@
       <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="38"/>
+      <c r="H8" s="42"/>
       <c r="Z8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1088,8 +1088,8 @@
       <c r="F9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
       <c r="Z9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1125,8 +1125,8 @@
       <c r="F10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -1147,8 +1147,8 @@
       <c r="F11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
@@ -1169,8 +1169,8 @@
       <c r="F12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1430,7 +1430,7 @@
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,35 +1440,35 @@
     <col min="3" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="39" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Tests by Weight to rate POST request functionality; and some additional refactoring to test wordings
</commit_message>
<xml_diff>
--- a/test/TestConditions.xlsx
+++ b/test/TestConditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96977D-BE29-4091-9FF4-BB193644AF2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D01C01-B530-4240-94F0-C48F07AFD0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
+    <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="34">
   <si>
     <t>Width</t>
   </si>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238D5791-8EED-4FC6-B7FB-0F4224317556}">
   <dimension ref="A1:AR29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>24</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>24</v>
@@ -1412,8 +1412,8 @@
       <c r="E29" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="14">
-        <v>0</v>
+      <c r="F29" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC910C0-C4E2-486F-90F5-9B3D69A286F7}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2056,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>24</v>
@@ -2702,7 +2702,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>24</v>
@@ -3604,7 +3604,7 @@
         <v>11</v>
       </c>
       <c r="G68" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="16" t="s">
         <v>24</v>
@@ -3638,8 +3638,8 @@
       <c r="G69" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H69" s="15">
-        <v>0</v>
+      <c r="H69" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="I69" s="5">
         <v>400</v>

</xml_diff>

<commit_message>
Document for first sections of deliverable
</commit_message>
<xml_diff>
--- a/test/TestConditions.xlsx
+++ b/test/TestConditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D01C01-B530-4240-94F0-C48F07AFD0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D13A19-8A60-484A-A486-8DCDB65816BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
+    <workbookView xWindow="38280" yWindow="-4215" windowWidth="16440" windowHeight="29040" activeTab="1" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="29">
   <si>
     <t>Width</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>Lengths:</t>
-  </si>
-  <si>
-    <t>Weights:</t>
-  </si>
-  <si>
-    <t>Validities:</t>
-  </si>
-  <si>
-    <t>Rates:</t>
-  </si>
-  <si>
-    <t>Widths</t>
   </si>
   <si>
     <t>Length_Unit</t>
@@ -712,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238D5791-8EED-4FC6-B7FB-0F4224317556}">
-  <dimension ref="A1:AR29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,50 +712,50 @@
     <col min="12" max="16384" width="7.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>-1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" s="12">
         <v>-1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" s="12">
         <v>-1</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
@@ -779,24 +764,24 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" s="18">
         <v>0</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" s="18">
         <v>0</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G3" s="12">
         <v>400</v>
@@ -805,451 +790,292 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" s="18">
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" s="18">
         <v>1</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="8">
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>139</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" s="18">
         <v>89</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5" s="18">
         <v>2</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="17">
         <v>2.4</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AB5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>139</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>140</v>
-      </c>
-      <c r="AF5" s="4">
-        <v>141</v>
-      </c>
-      <c r="AG5" s="4">
-        <v>244</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>245</v>
-      </c>
-      <c r="AI5" s="4">
-        <v>246</v>
-      </c>
-      <c r="AJ5" s="4">
-        <v>379</v>
-      </c>
-      <c r="AK5" s="4">
-        <v>380</v>
-      </c>
-      <c r="AL5" s="4">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>140</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>90</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AB6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>89</v>
-      </c>
-      <c r="AE6" s="4">
-        <v>90</v>
-      </c>
-      <c r="AF6" s="4">
-        <v>91</v>
-      </c>
-      <c r="AG6" s="4">
-        <v>155</v>
-      </c>
-      <c r="AH6" s="4">
-        <v>156</v>
-      </c>
-      <c r="AI6" s="4">
-        <v>157</v>
-      </c>
-      <c r="AJ6" s="4">
-        <v>269</v>
-      </c>
-      <c r="AK6" s="4">
-        <v>270</v>
-      </c>
-      <c r="AL6" s="4">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>141</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>91</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H7" s="41"/>
-      <c r="Z7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AB7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE7" s="4">
-        <v>3</v>
-      </c>
-      <c r="AF7" s="4">
-        <v>4</v>
-      </c>
-      <c r="AG7" s="4">
-        <v>29</v>
-      </c>
-      <c r="AH7" s="4">
-        <v>30</v>
-      </c>
-      <c r="AI7" s="4">
-        <v>31</v>
-      </c>
-      <c r="AJ7" s="4">
-        <v>49</v>
-      </c>
-      <c r="AK7" s="4">
-        <v>50</v>
-      </c>
-      <c r="AL7" s="4">
-        <v>51</v>
-      </c>
-      <c r="AM7" s="4">
-        <v>99</v>
-      </c>
-      <c r="AN7" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO7" s="4">
-        <v>101</v>
-      </c>
-      <c r="AP7" s="4">
-        <v>499</v>
-      </c>
-      <c r="AQ7" s="4">
-        <v>500</v>
-      </c>
-      <c r="AR7" s="4">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>244</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>155</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1">
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="42" t="s">
-        <v>19</v>
-      </c>
       <c r="H8" s="42"/>
-      <c r="Z8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" s="4">
-        <v>200</v>
-      </c>
-      <c r="AB8" s="4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>245</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>156</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
-      <c r="Z9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA9" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="AB9" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="AC9" s="4">
-        <v>0.98</v>
-      </c>
-      <c r="AD9" s="4">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>246</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C10" s="18">
         <v>157</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E10" s="22">
         <v>31</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>379</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11" s="18">
         <v>269</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E11" s="22">
         <v>49</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>380</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12" s="18">
         <v>270</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E12" s="22">
         <v>50</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>381</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13" s="12">
         <v>271</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E13" s="18">
         <v>51</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>-1</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C14" s="12">
         <v>-1</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E14" s="18">
         <v>99</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C15" s="18">
         <v>0</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E15" s="18">
         <v>100</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>1</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C16" s="18">
         <v>1</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E16" s="24">
         <v>101</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,19 +1083,19 @@
         <v>7.875</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E17" s="24">
         <v>499</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,19 +1103,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C18" s="18">
         <v>8</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E18" s="24">
         <v>500</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1297,19 +1123,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C19" s="12">
         <v>12</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E19" s="12">
         <v>501</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,39 +1143,39 @@
         <v>1</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E20" s="12">
         <v>-1</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E21" s="18">
         <v>0</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,7 +1183,7 @@
         <v>0.5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1373,7 +1199,7 @@
         <v>1.5</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1381,7 +1207,7 @@
         <v>2.5</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,7 +1215,7 @@
         <v>9</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,7 +1223,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1405,15 +1231,15 @@
         <v>1</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1429,52 +1255,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC910C0-C4E2-486F-90F5-9B3D69A286F7}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="H1" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="J1" s="39" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1483,30 +1316,30 @@
         <v>-1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4">
         <v>125</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G2" s="9">
         <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I2" s="4">
         <v>400</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -1515,19 +1348,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" s="4">
         <v>125</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G3" s="9">
         <v>15</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I3" s="4">
         <v>200</v>
@@ -1538,7 +1371,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
@@ -1547,19 +1380,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4">
         <v>125</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G4" s="9">
         <v>15</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I4" s="4">
         <v>200</v>
@@ -1570,7 +1403,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -1579,19 +1412,19 @@
         <v>139</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4">
         <v>125</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G5" s="9">
         <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I5" s="4">
         <v>200</v>
@@ -1602,7 +1435,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
@@ -1611,19 +1444,19 @@
         <v>140</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6" s="4">
         <v>125</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9">
         <v>15</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I6" s="4">
         <v>200</v>
@@ -1634,7 +1467,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
@@ -1643,19 +1476,19 @@
         <v>141</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4">
         <v>125</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G7" s="9">
         <v>15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I7" s="4">
         <v>200</v>
@@ -1666,7 +1499,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
@@ -1675,19 +1508,19 @@
         <v>244</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E8" s="4">
         <v>125</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G8" s="9">
         <v>15</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I8" s="4">
         <v>200</v>
@@ -1698,7 +1531,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
@@ -1707,19 +1540,19 @@
         <v>245</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4">
         <v>125</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G9" s="9">
         <v>15</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I9" s="4">
         <v>200</v>
@@ -1730,7 +1563,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
@@ -1739,19 +1572,19 @@
         <v>246</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E10" s="4">
         <v>125</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G10" s="9">
         <v>15</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I10" s="4">
         <v>200</v>
@@ -1762,7 +1595,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
@@ -1771,19 +1604,19 @@
         <v>379</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E11" s="4">
         <v>125</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G11" s="9">
         <v>15</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I11" s="4">
         <v>200</v>
@@ -1794,7 +1627,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
@@ -1803,19 +1636,19 @@
         <v>380</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4">
         <v>125</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G12" s="9">
         <v>15</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I12" s="4">
         <v>200</v>
@@ -1826,7 +1659,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
@@ -1835,30 +1668,30 @@
         <v>381</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E13" s="4">
         <v>125</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G13" s="9">
         <v>15</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I13" s="4">
         <v>400</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
@@ -1867,30 +1700,30 @@
         <v>-1</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4">
         <v>125</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G14" s="9">
         <v>15</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I14" s="4">
         <v>400</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
@@ -1899,19 +1732,19 @@
         <v>0</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4">
         <v>125</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G15" s="9">
         <v>15</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I15" s="9">
         <v>200</v>
@@ -1922,7 +1755,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
@@ -1931,19 +1764,19 @@
         <v>1</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E16" s="4">
         <v>125</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G16" s="9">
         <v>15</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I16" s="9">
         <v>200</v>
@@ -1954,7 +1787,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4">
         <v>16</v>
@@ -1963,19 +1796,19 @@
         <v>7.875</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E17" s="4">
         <v>125</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9">
         <v>15</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I17" s="9">
         <v>200</v>
@@ -1986,7 +1819,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" s="4">
         <v>17</v>
@@ -1995,19 +1828,19 @@
         <v>12</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4">
         <v>125</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G18" s="9">
         <v>15</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I18" s="9">
         <v>200</v>
@@ -2018,7 +1851,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4">
         <v>18</v>
@@ -2027,30 +1860,30 @@
         <v>16</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4">
         <v>125</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G19" s="9">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I19" s="4">
         <v>400</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -2059,62 +1892,62 @@
         <v>1</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E20" s="4">
         <v>125</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G20" s="9">
         <v>15</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4">
         <v>400</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E21" s="4">
         <v>125</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G21" s="9">
         <v>15</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I21" s="4">
         <v>400</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4">
         <v>21</v>
@@ -2123,30 +1956,30 @@
         <v>200</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E22" s="16">
         <v>-1</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G22" s="9">
         <v>15</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I22" s="4">
         <v>400</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4">
         <v>22</v>
@@ -2155,19 +1988,19 @@
         <v>200</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E23" s="26">
         <v>0</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G23" s="9">
         <v>15</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I23" s="9">
         <v>200</v>
@@ -2178,7 +2011,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B24" s="4">
         <v>23</v>
@@ -2187,19 +2020,19 @@
         <v>200</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E24" s="26">
         <v>1</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G24" s="9">
         <v>15</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I24" s="9">
         <v>200</v>
@@ -2210,7 +2043,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
@@ -2219,19 +2052,19 @@
         <v>200</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E25" s="26">
         <v>89</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G25" s="9">
         <v>15</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I25" s="9">
         <v>200</v>
@@ -2242,7 +2075,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26" s="4">
         <v>25</v>
@@ -2251,19 +2084,19 @@
         <v>200</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E26" s="4">
         <v>90</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G26" s="9">
         <v>15</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I26" s="9">
         <v>200</v>
@@ -2274,7 +2107,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B27" s="4">
         <v>26</v>
@@ -2283,19 +2116,19 @@
         <v>200</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E27" s="4">
         <v>91</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G27" s="9">
         <v>15</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I27" s="9">
         <v>200</v>
@@ -2306,7 +2139,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4">
         <v>27</v>
@@ -2315,19 +2148,19 @@
         <v>200</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4">
         <v>155</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G28" s="9">
         <v>15</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I28" s="9">
         <v>200</v>
@@ -2338,7 +2171,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4">
         <v>28</v>
@@ -2347,19 +2180,19 @@
         <v>200</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E29" s="4">
         <v>156</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G29" s="9">
         <v>15</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I29" s="9">
         <v>200</v>
@@ -2370,7 +2203,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B30" s="4">
         <v>29</v>
@@ -2379,19 +2212,19 @@
         <v>200</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E30" s="26">
         <v>157</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G30" s="9">
         <v>15</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I30" s="9">
         <v>200</v>
@@ -2402,7 +2235,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B31" s="4">
         <v>30</v>
@@ -2411,19 +2244,19 @@
         <v>200</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E31" s="26">
         <v>269</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G31" s="9">
         <v>15</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I31" s="9">
         <v>200</v>
@@ -2434,7 +2267,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B32" s="4">
         <v>31</v>
@@ -2443,19 +2276,19 @@
         <v>200</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E32" s="26">
         <v>270</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G32" s="9">
         <v>15</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I32" s="9">
         <v>200</v>
@@ -2466,7 +2299,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B33" s="4">
         <v>32</v>
@@ -2475,30 +2308,30 @@
         <v>200</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E33" s="16">
         <v>271</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G33" s="9">
         <v>15</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I33" s="4">
         <v>400</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B34" s="4">
         <v>33</v>
@@ -2507,30 +2340,30 @@
         <v>200</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E34" s="16">
         <v>-1</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G34" s="9">
         <v>15</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I34" s="4">
         <v>400</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B35" s="4">
         <v>34</v>
@@ -2539,19 +2372,19 @@
         <v>200</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E35" s="26">
         <v>0</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G35" s="9">
         <v>15</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I35" s="9">
         <v>200</v>
@@ -2562,7 +2395,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -2571,19 +2404,19 @@
         <v>200</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E36" s="26">
         <v>1</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G36" s="9">
         <v>15</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I36" s="9">
         <v>200</v>
@@ -2594,7 +2427,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B37" s="4">
         <v>36</v>
@@ -2603,19 +2436,19 @@
         <v>200</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E37" s="4">
         <v>5</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G37" s="9">
         <v>15</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I37" s="9">
         <v>200</v>
@@ -2626,7 +2459,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B38" s="4">
         <v>37</v>
@@ -2635,19 +2468,19 @@
         <v>200</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E38" s="26">
         <v>8</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G38" s="9">
         <v>15</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I38" s="9">
         <v>200</v>
@@ -2658,7 +2491,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B39" s="4">
         <v>38</v>
@@ -2667,30 +2500,30 @@
         <v>200</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E39" s="16">
         <v>12</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G39" s="9">
         <v>15</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I39" s="4">
         <v>400</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B40" s="4">
         <v>39</v>
@@ -2699,30 +2532,30 @@
         <v>200</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E40" s="16">
         <v>1</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G40" s="9">
         <v>15</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I40" s="4">
         <v>400</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B41" s="4">
         <v>40</v>
@@ -2731,30 +2564,30 @@
         <v>200</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G41" s="9">
         <v>15</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I41" s="4">
         <v>400</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B42" s="4">
         <v>41</v>
@@ -2763,30 +2596,30 @@
         <v>200</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E42" s="4">
         <v>125</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G42" s="16">
         <v>-1</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I42" s="4">
         <v>400</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B43" s="4">
         <v>42</v>
@@ -2795,19 +2628,19 @@
         <v>200</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E43" s="4">
         <v>125</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G43" s="26">
         <v>0</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I43" s="9">
         <v>200</v>
@@ -2818,7 +2651,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B44" s="4">
         <v>43</v>
@@ -2827,19 +2660,19 @@
         <v>200</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E44" s="4">
         <v>125</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G44" s="26">
         <v>1</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I44" s="9">
         <v>200</v>
@@ -2850,7 +2683,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B45" s="4">
         <v>44</v>
@@ -2859,19 +2692,19 @@
         <v>200</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E45" s="4">
         <v>125</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G45" s="26">
         <v>2</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I45" s="9">
         <v>200</v>
@@ -2882,7 +2715,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B46" s="4">
         <v>45</v>
@@ -2891,19 +2724,19 @@
         <v>200</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E46" s="4">
         <v>125</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G46" s="4">
         <v>3</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I46" s="9">
         <v>200</v>
@@ -2914,7 +2747,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B47" s="4">
         <v>46</v>
@@ -2923,19 +2756,19 @@
         <v>200</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E47" s="4">
         <v>125</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G47" s="4">
         <v>4</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I47" s="9">
         <v>200</v>
@@ -2946,7 +2779,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B48" s="4">
         <v>47</v>
@@ -2955,19 +2788,19 @@
         <v>200</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E48" s="4">
         <v>125</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G48" s="4">
         <v>29</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I48" s="9">
         <v>200</v>
@@ -2978,7 +2811,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B49" s="4">
         <v>48</v>
@@ -2987,19 +2820,19 @@
         <v>200</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E49" s="4">
         <v>125</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G49" s="4">
         <v>30</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I49" s="9">
         <v>200</v>
@@ -3010,7 +2843,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B50" s="4">
         <v>49</v>
@@ -3019,19 +2852,19 @@
         <v>200</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E50" s="4">
         <v>125</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G50" s="27">
         <v>31</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I50" s="9">
         <v>200</v>
@@ -3042,7 +2875,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B51" s="4">
         <v>50</v>
@@ -3051,19 +2884,19 @@
         <v>200</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E51" s="4">
         <v>125</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G51" s="27">
         <v>49</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I51" s="9">
         <v>200</v>
@@ -3074,7 +2907,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B52" s="4">
         <v>51</v>
@@ -3083,19 +2916,19 @@
         <v>200</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E52" s="4">
         <v>125</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G52" s="27">
         <v>50</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I52" s="9">
         <v>200</v>
@@ -3106,7 +2939,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B53" s="4">
         <v>52</v>
@@ -3115,19 +2948,19 @@
         <v>200</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E53" s="4">
         <v>125</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G53" s="26">
         <v>51</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I53" s="9">
         <v>200</v>
@@ -3138,7 +2971,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B54" s="4">
         <v>53</v>
@@ -3147,19 +2980,19 @@
         <v>200</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E54" s="4">
         <v>125</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G54" s="26">
         <v>99</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I54" s="9">
         <v>200</v>
@@ -3170,7 +3003,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B55" s="4">
         <v>54</v>
@@ -3179,19 +3012,19 @@
         <v>200</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E55" s="4">
         <v>125</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G55" s="26">
         <v>100</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I55" s="9">
         <v>200</v>
@@ -3202,7 +3035,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
@@ -3211,19 +3044,19 @@
         <v>200</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E56" s="4">
         <v>125</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G56" s="28">
         <v>101</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I56" s="9">
         <v>200</v>
@@ -3234,7 +3067,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B57" s="4">
         <v>56</v>
@@ -3243,19 +3076,19 @@
         <v>200</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E57" s="4">
         <v>125</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G57" s="28">
         <v>499</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I57" s="9">
         <v>200</v>
@@ -3266,7 +3099,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B58" s="4">
         <v>57</v>
@@ -3275,19 +3108,19 @@
         <v>200</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E58" s="4">
         <v>125</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G58" s="28">
         <v>500</v>
       </c>
       <c r="H58" s="28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I58" s="9">
         <v>200</v>
@@ -3298,7 +3131,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
@@ -3307,30 +3140,30 @@
         <v>200</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E59" s="4">
         <v>125</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G59" s="16">
         <v>501</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I59" s="4">
         <v>400</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B60" s="4">
         <v>59</v>
@@ -3339,30 +3172,30 @@
         <v>200</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E60" s="4">
         <v>125</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G60" s="16">
         <v>-1</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I60" s="4">
         <v>400</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B61" s="4">
         <v>60</v>
@@ -3371,19 +3204,19 @@
         <v>200</v>
       </c>
       <c r="D61" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E61" s="4">
         <v>125</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G61" s="26">
         <v>0</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I61" s="9">
         <v>200</v>
@@ -3394,7 +3227,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B62" s="4">
         <v>61</v>
@@ -3403,19 +3236,19 @@
         <v>200</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E62" s="4">
         <v>125</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G62" s="4">
         <v>0.5</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I62" s="9">
         <v>200</v>
@@ -3426,7 +3259,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B63" s="4">
         <v>62</v>
@@ -3435,19 +3268,19 @@
         <v>200</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E63" s="4">
         <v>125</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G63" s="4">
         <v>1</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I63" s="9">
         <v>200</v>
@@ -3458,7 +3291,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B64" s="4">
         <v>63</v>
@@ -3467,19 +3300,19 @@
         <v>200</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E64" s="4">
         <v>125</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G64" s="27">
         <v>1.5</v>
       </c>
       <c r="H64" s="27" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I64" s="9">
         <v>200</v>
@@ -3490,7 +3323,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B65" s="4">
         <v>64</v>
@@ -3499,19 +3332,19 @@
         <v>200</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E65" s="4">
         <v>125</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G65" s="26">
         <v>2.5</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I65" s="9">
         <v>200</v>
@@ -3522,7 +3355,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B66" s="4">
         <v>65</v>
@@ -3531,19 +3364,19 @@
         <v>200</v>
       </c>
       <c r="D66" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="4">
+        <v>125</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="28">
+        <v>9</v>
+      </c>
+      <c r="H66" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="E66" s="4">
-        <v>125</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G66" s="28">
-        <v>9</v>
-      </c>
-      <c r="H66" s="28" t="s">
-        <v>16</v>
       </c>
       <c r="I66" s="9">
         <v>200</v>
@@ -3554,7 +3387,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B67" s="4">
         <v>66</v>
@@ -3563,30 +3396,30 @@
         <v>200</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E67" s="4">
         <v>125</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G67" s="16">
         <v>20</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I67" s="4">
         <v>400</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B68" s="4">
         <v>67</v>
@@ -3595,30 +3428,30 @@
         <v>200</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E68" s="4">
         <v>125</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G68" s="16">
         <v>1</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I68" s="4">
         <v>400</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B69" s="5">
         <v>68</v>
@@ -3627,25 +3460,25 @@
         <v>200</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E69" s="5">
         <v>125</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G69" s="36" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I69" s="5">
         <v>400</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>